<commit_message>
Paper revision. Changes in the ontology and adding NCBI sample identifiers
</commit_message>
<xml_diff>
--- a/data/ontology/2023-12-21_mfd-habitat-ontology.xlsx
+++ b/data/ontology/2023-12-21_mfd-habitat-ontology.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1582" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1586" uniqueCount="285">
   <si>
     <t xml:space="preserve">mfd_sampletype</t>
   </si>
@@ -1131,7 +1131,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A198" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A231" activeCellId="0" sqref="A231"/>
+      <selection pane="topLeft" activeCell="E226" activeCellId="0" sqref="E226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7995,12 +7995,8 @@
       <c r="D226" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E226" s="12" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F226" s="12" t="s">
-        <v>212</v>
-      </c>
+      <c r="E226" s="12"/>
+      <c r="F226" s="12"/>
       <c r="G226" s="12"/>
       <c r="H226" s="12"/>
       <c r="I226" s="12"/>
@@ -8027,12 +8023,8 @@
       <c r="F227" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="G227" s="12" t="n">
-        <v>1110</v>
-      </c>
-      <c r="H227" s="12" t="s">
-        <v>251</v>
-      </c>
+      <c r="G227" s="12"/>
+      <c r="H227" s="12"/>
       <c r="I227" s="12"/>
       <c r="K227" s="0" t="s">
         <v>228</v>
@@ -8058,14 +8050,14 @@
         <v>212</v>
       </c>
       <c r="G228" s="12" t="n">
-        <v>1120</v>
+        <v>1110</v>
       </c>
       <c r="H228" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I228" s="12"/>
       <c r="K228" s="0" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8082,13 +8074,17 @@
         <v>211</v>
       </c>
       <c r="E229" s="12" t="n">
-        <v>1200</v>
+        <v>1100</v>
       </c>
       <c r="F229" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="G229" s="12"/>
-      <c r="H229" s="12"/>
+        <v>212</v>
+      </c>
+      <c r="G229" s="12" t="n">
+        <v>1120</v>
+      </c>
+      <c r="H229" s="12" t="s">
+        <v>252</v>
+      </c>
       <c r="I229" s="12"/>
       <c r="K229" s="0" t="s">
         <v>253</v>
@@ -8113,12 +8109,8 @@
       <c r="F230" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="G230" s="12" t="n">
-        <v>1210</v>
-      </c>
-      <c r="H230" s="12" t="s">
-        <v>255</v>
-      </c>
+      <c r="G230" s="12"/>
+      <c r="H230" s="12"/>
       <c r="I230" s="12"/>
       <c r="K230" s="0" t="s">
         <v>253</v>
@@ -8144,10 +8136,10 @@
         <v>254</v>
       </c>
       <c r="G231" s="12" t="n">
-        <v>1220</v>
+        <v>1210</v>
       </c>
       <c r="H231" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I231" s="12"/>
       <c r="K231" s="0" t="s">
@@ -8174,10 +8166,10 @@
         <v>254</v>
       </c>
       <c r="G232" s="12" t="n">
-        <v>1230</v>
+        <v>1220</v>
       </c>
       <c r="H232" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I232" s="12"/>
       <c r="K232" s="0" t="s">
@@ -8198,13 +8190,17 @@
         <v>211</v>
       </c>
       <c r="E233" s="12" t="n">
-        <v>1300</v>
+        <v>1200</v>
       </c>
       <c r="F233" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="G233" s="12"/>
-      <c r="H233" s="12"/>
+        <v>254</v>
+      </c>
+      <c r="G233" s="12" t="n">
+        <v>1230</v>
+      </c>
+      <c r="H233" s="12" t="s">
+        <v>257</v>
+      </c>
       <c r="I233" s="12"/>
       <c r="K233" s="0" t="s">
         <v>253</v>
@@ -8229,12 +8225,8 @@
       <c r="F234" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="G234" s="12" t="n">
-        <v>1310</v>
-      </c>
-      <c r="H234" s="12" t="s">
-        <v>258</v>
-      </c>
+      <c r="G234" s="12"/>
+      <c r="H234" s="12"/>
       <c r="I234" s="12"/>
       <c r="K234" s="0" t="s">
         <v>253</v>
@@ -8254,16 +8246,16 @@
         <v>211</v>
       </c>
       <c r="E235" s="12" t="n">
-        <v>1400</v>
+        <v>1300</v>
       </c>
       <c r="F235" s="12" t="s">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="G235" s="12" t="n">
-        <v>1410</v>
+        <v>1310</v>
       </c>
       <c r="H235" s="12" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I235" s="12"/>
       <c r="K235" s="0" t="s">
@@ -8290,10 +8282,10 @@
         <v>259</v>
       </c>
       <c r="G236" s="12" t="n">
-        <v>1420</v>
+        <v>1410</v>
       </c>
       <c r="H236" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I236" s="12"/>
       <c r="K236" s="0" t="s">
@@ -8302,10 +8294,10 @@
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="12" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="B237" s="12" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="C237" s="12" t="n">
         <v>1000</v>
@@ -8313,13 +8305,21 @@
       <c r="D237" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E237" s="12"/>
-      <c r="F237" s="12"/>
-      <c r="G237" s="12"/>
-      <c r="H237" s="12"/>
+      <c r="E237" s="12" t="n">
+        <v>1400</v>
+      </c>
+      <c r="F237" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="G237" s="12" t="n">
+        <v>1420</v>
+      </c>
+      <c r="H237" s="12" t="s">
+        <v>261</v>
+      </c>
       <c r="I237" s="12"/>
       <c r="K237" s="0" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8335,12 +8335,8 @@
       <c r="D238" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E238" s="12" t="n">
-        <v>1100</v>
-      </c>
-      <c r="F238" s="12" t="s">
-        <v>264</v>
-      </c>
+      <c r="E238" s="12"/>
+      <c r="F238" s="12"/>
       <c r="G238" s="12"/>
       <c r="H238" s="12"/>
       <c r="I238" s="12"/>
@@ -8362,10 +8358,10 @@
         <v>211</v>
       </c>
       <c r="E239" s="12" t="n">
-        <v>1300</v>
+        <v>1100</v>
       </c>
       <c r="F239" s="12" t="s">
-        <v>223</v>
+        <v>264</v>
       </c>
       <c r="G239" s="12"/>
       <c r="H239" s="12"/>
@@ -8379,25 +8375,25 @@
         <v>262</v>
       </c>
       <c r="B240" s="12" t="s">
-        <v>202</v>
+        <v>12</v>
       </c>
       <c r="C240" s="12" t="n">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="D240" s="12" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="E240" s="12" t="n">
-        <v>3100</v>
+        <v>1300</v>
       </c>
       <c r="F240" s="12" t="s">
-        <v>265</v>
+        <v>223</v>
       </c>
       <c r="G240" s="12"/>
       <c r="H240" s="12"/>
       <c r="I240" s="12"/>
-      <c r="K240" s="4" t="s">
-        <v>266</v>
+      <c r="K240" s="0" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8419,12 +8415,8 @@
       <c r="F241" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="G241" s="12" t="n">
-        <v>3110</v>
-      </c>
-      <c r="H241" s="12" t="s">
-        <v>267</v>
-      </c>
+      <c r="G241" s="12"/>
+      <c r="H241" s="12"/>
       <c r="I241" s="12"/>
       <c r="K241" s="4" t="s">
         <v>266</v>
@@ -8450,10 +8442,10 @@
         <v>265</v>
       </c>
       <c r="G242" s="12" t="n">
-        <v>3120</v>
+        <v>3110</v>
       </c>
       <c r="H242" s="12" t="s">
-        <v>204</v>
+        <v>267</v>
       </c>
       <c r="I242" s="12"/>
       <c r="K242" s="4" t="s">
@@ -8480,10 +8472,10 @@
         <v>265</v>
       </c>
       <c r="G243" s="12" t="n">
-        <v>3130</v>
+        <v>3120</v>
       </c>
       <c r="H243" s="12" t="s">
-        <v>268</v>
+        <v>204</v>
       </c>
       <c r="I243" s="12"/>
       <c r="K243" s="4" t="s">
@@ -8510,10 +8502,10 @@
         <v>265</v>
       </c>
       <c r="G244" s="12" t="n">
-        <v>3140</v>
+        <v>3130</v>
       </c>
       <c r="H244" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I244" s="12"/>
       <c r="K244" s="4" t="s">
@@ -8525,18 +8517,28 @@
         <v>262</v>
       </c>
       <c r="B245" s="12" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="C245" s="12" t="n">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="D245" s="12" t="s">
-        <v>270</v>
-      </c>
-      <c r="E245" s="12"/>
-      <c r="F245" s="12"/>
+        <v>227</v>
+      </c>
+      <c r="E245" s="12" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F245" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="G245" s="12" t="n">
+        <v>3140</v>
+      </c>
+      <c r="H245" s="12" t="s">
+        <v>269</v>
+      </c>
       <c r="I245" s="12"/>
-      <c r="K245" s="0" t="s">
+      <c r="K245" s="4" t="s">
         <v>266</v>
       </c>
     </row>
@@ -8548,10 +8550,10 @@
         <v>193</v>
       </c>
       <c r="C246" s="12" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="D246" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E246" s="12"/>
       <c r="F246" s="12"/>
@@ -8573,12 +8575,8 @@
       <c r="D247" s="12" t="s">
         <v>271</v>
       </c>
-      <c r="E247" s="12" t="n">
-        <v>2100</v>
-      </c>
-      <c r="F247" s="12" t="s">
-        <v>272</v>
-      </c>
+      <c r="E247" s="12"/>
+      <c r="F247" s="12"/>
       <c r="I247" s="12"/>
       <c r="K247" s="0" t="s">
         <v>266</v>
@@ -8598,10 +8596,10 @@
         <v>271</v>
       </c>
       <c r="E248" s="12" t="n">
-        <v>2200</v>
+        <v>2100</v>
       </c>
       <c r="F248" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I248" s="12"/>
       <c r="K248" s="0" t="s">
@@ -8616,13 +8614,17 @@
         <v>193</v>
       </c>
       <c r="C249" s="12" t="n">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="D249" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="E249" s="12"/>
-      <c r="F249" s="12"/>
+        <v>271</v>
+      </c>
+      <c r="E249" s="12" t="n">
+        <v>2200</v>
+      </c>
+      <c r="F249" s="12" t="s">
+        <v>273</v>
+      </c>
       <c r="I249" s="12"/>
       <c r="K249" s="0" t="s">
         <v>266</v>
@@ -8641,12 +8643,8 @@
       <c r="D250" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="E250" s="12" t="n">
-        <v>5100</v>
-      </c>
-      <c r="F250" s="12" t="s">
-        <v>198</v>
-      </c>
+      <c r="E250" s="12"/>
+      <c r="F250" s="12"/>
       <c r="I250" s="12"/>
       <c r="K250" s="0" t="s">
         <v>266</v>
@@ -8660,14 +8658,21 @@
         <v>193</v>
       </c>
       <c r="C251" s="12" t="n">
-        <v>4000</v>
+        <v>5000</v>
       </c>
       <c r="D251" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="E251" s="12"/>
-      <c r="F251" s="12"/>
+        <v>197</v>
+      </c>
+      <c r="E251" s="12" t="n">
+        <v>5100</v>
+      </c>
+      <c r="F251" s="12" t="s">
+        <v>198</v>
+      </c>
       <c r="I251" s="12"/>
+      <c r="K251" s="0" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A252" s="12" t="s">
@@ -8682,12 +8687,8 @@
       <c r="D252" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="E252" s="12" t="n">
-        <v>4100</v>
-      </c>
-      <c r="F252" s="12" t="s">
-        <v>275</v>
-      </c>
+      <c r="E252" s="12"/>
+      <c r="F252" s="12"/>
       <c r="I252" s="12"/>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8704,10 +8705,10 @@
         <v>274</v>
       </c>
       <c r="E253" s="12" t="n">
-        <v>4200</v>
+        <v>4100</v>
       </c>
       <c r="F253" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I253" s="12"/>
     </row>
@@ -8725,10 +8726,10 @@
         <v>274</v>
       </c>
       <c r="E254" s="12" t="n">
-        <v>4300</v>
+        <v>4200</v>
       </c>
       <c r="F254" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I254" s="12"/>
     </row>
@@ -8740,14 +8741,18 @@
         <v>193</v>
       </c>
       <c r="C255" s="12" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D255" s="14" t="s">
-        <v>278</v>
-      </c>
-      <c r="K255" s="0" t="s">
-        <v>266</v>
-      </c>
+        <v>4000</v>
+      </c>
+      <c r="D255" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="E255" s="12" t="n">
+        <v>4300</v>
+      </c>
+      <c r="F255" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="I255" s="12"/>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A256" s="12" t="s">
@@ -8762,15 +8767,6 @@
       <c r="D256" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="E256" s="14" t="n">
-        <v>3300</v>
-      </c>
-      <c r="F256" s="14" t="s">
-        <v>279</v>
-      </c>
-      <c r="G256" s="14"/>
-      <c r="H256" s="14"/>
-      <c r="I256" s="14"/>
       <c r="K256" s="0" t="s">
         <v>266</v>
       </c>
@@ -8789,10 +8785,10 @@
         <v>278</v>
       </c>
       <c r="E257" s="14" t="n">
-        <v>3100</v>
+        <v>3300</v>
       </c>
       <c r="F257" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G257" s="14"/>
       <c r="H257" s="14"/>
@@ -8820,12 +8816,8 @@
       <c r="F258" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="G258" s="14" t="n">
-        <v>3110</v>
-      </c>
-      <c r="H258" s="14" t="s">
-        <v>281</v>
-      </c>
+      <c r="G258" s="14"/>
+      <c r="H258" s="14"/>
       <c r="I258" s="14"/>
       <c r="K258" s="0" t="s">
         <v>266</v>
@@ -8851,10 +8843,10 @@
         <v>280</v>
       </c>
       <c r="G259" s="14" t="n">
-        <v>3120</v>
+        <v>3110</v>
       </c>
       <c r="H259" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I259" s="14"/>
       <c r="K259" s="0" t="s">
@@ -8881,10 +8873,10 @@
         <v>280</v>
       </c>
       <c r="G260" s="14" t="n">
-        <v>3130</v>
+        <v>3120</v>
       </c>
       <c r="H260" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I260" s="14"/>
       <c r="K260" s="0" t="s">
@@ -8911,10 +8903,10 @@
         <v>280</v>
       </c>
       <c r="G261" s="14" t="n">
-        <v>3140</v>
+        <v>3130</v>
       </c>
       <c r="H261" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I261" s="14"/>
       <c r="K261" s="0" t="s">
@@ -8922,11 +8914,40 @@
       </c>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A262" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="B262" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C262" s="12" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D262" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="E262" s="14" t="n">
+        <v>3100</v>
+      </c>
+      <c r="F262" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="G262" s="14" t="n">
+        <v>3140</v>
+      </c>
+      <c r="H262" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="I262" s="14"/>
       <c r="K262" s="0" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K263" s="0" t="s">
+        <v>266</v>
+      </c>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>